<commit_message>
Working HashRouter & ServicePage
</commit_message>
<xml_diff>
--- a/tabels.xlsx
+++ b/tabels.xlsx
@@ -253,7 +253,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,6 +300,14 @@
       <family val="3"/>
       <charset val="238"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Inconsolata"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -333,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -358,6 +366,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -663,7 +674,7 @@
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -674,13 +685,13 @@
     <col min="4" max="5" width="9.140625" style="2"/>
     <col min="6" max="6" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="8" style="2" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" style="2" customWidth="1"/>
     <col min="9" max="9" width="12.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.140625" style="2" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.28515625" style="2" customWidth="1"/>
     <col min="16" max="16" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.140625" style="2" bestFit="1" customWidth="1"/>
@@ -969,22 +980,22 @@
       <c r="R6" s="4"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="B7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="E7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>3</v>
       </c>
       <c r="H7" s="4">
@@ -1061,37 +1072,37 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="M9" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="N9" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="O9" s="4" t="s">
+      <c r="O9" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="P9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q9" s="4" t="s">
+      <c r="P9" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="R9" s="4" t="s">
+      <c r="R9" s="9" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1164,10 +1175,10 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="9" t="s">
         <v>3</v>
       </c>
       <c r="H15" s="4">
@@ -1255,19 +1266,19 @@
       <c r="C19" s="4">
         <v>1</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H19" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="J19" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="K19" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="L19" s="4" t="s">
+      <c r="L19" s="9" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1305,13 +1316,13 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="4" t="s">
+      <c r="B23" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
After tests; Dosn't work; Lots to fix and improve;
</commit_message>
<xml_diff>
--- a/tabels.xlsx
+++ b/tabels.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="87">
   <si>
     <t>mba_id</t>
   </si>
@@ -247,13 +247,43 @@
   </si>
   <si>
     <t>oco_id</t>
+  </si>
+  <si>
+    <t>TO DO</t>
+  </si>
+  <si>
+    <t>#1</t>
+  </si>
+  <si>
+    <t>Service Page - podział na zadania (linki do poszczególnych zadań)</t>
+  </si>
+  <si>
+    <t>#2</t>
+  </si>
+  <si>
+    <t>Service Page - kooperator - tabela z danymi + dodanie nowego</t>
+  </si>
+  <si>
+    <t>#3</t>
+  </si>
+  <si>
+    <t>Service Page - kooperator - edycja kooperatora</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>DELETE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,53 +293,61 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Inconsolata"/>
-      <family val="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="238"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Inconsolata"/>
-      <family val="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="238"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="Inconsolata"/>
-      <family val="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="238"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
-      <color theme="0"/>
-      <name val="Inconsolata"/>
-      <family val="3"/>
-      <charset val="238"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="0"/>
-      <name val="Inconsolata"/>
-      <family val="3"/>
-      <charset val="238"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color theme="1" tint="0.34998626667073579"/>
-      <name val="Inconsolata"/>
-      <family val="3"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -328,6 +366,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -341,34 +385,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -671,13 +718,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R36"/>
+  <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" style="2" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="2" customWidth="1"/>
@@ -980,22 +1027,22 @@
       <c r="R6" s="4"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="9" t="s">
+      <c r="B7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="9" t="s">
+      <c r="E7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H7" s="4">
@@ -1072,37 +1119,37 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="K9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="L9" s="9" t="s">
+      <c r="L9" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="M9" s="9" t="s">
+      <c r="M9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="N9" s="9" t="s">
+      <c r="N9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O9" s="9" t="s">
+      <c r="O9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="P9" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q9" s="9" t="s">
+      <c r="P9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="R9" s="9" t="s">
+      <c r="R9" s="6" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1113,7 +1160,7 @@
       <c r="B10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="7" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1124,7 +1171,7 @@
       <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="7" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1175,10 +1222,10 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H15" s="4">
@@ -1266,19 +1313,19 @@
       <c r="C19" s="4">
         <v>1</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="H19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I19" s="9" t="s">
+      <c r="I19" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J19" s="9" t="s">
+      <c r="J19" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="K19" s="9" t="s">
+      <c r="K19" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L19" s="9" t="s">
+      <c r="L19" s="6" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1316,34 +1363,34 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="9" t="s">
+      <c r="B23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
@@ -1361,7 +1408,7 @@
         <v>64</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>62</v>
@@ -1383,7 +1430,7 @@
         <v>67</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>65</v>
@@ -1405,24 +1452,24 @@
         <v>70</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>72</v>
       </c>
@@ -1433,7 +1480,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>74</v>
       </c>
@@ -1444,7 +1491,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>75</v>
       </c>
@@ -1453,6 +1500,38 @@
       </c>
       <c r="E36" s="2" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>